<commit_message>
fix: improve SSH command execution with pagination handling and case-insensitive serial search
</commit_message>
<xml_diff>
--- a/ONUs_migracao.xlsx
+++ b/ONUs_migracao.xlsx
@@ -1,56 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\ONU-TERMINATOR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>serial</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,48 +46,98 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -148,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,10 +211,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,7 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -391,24 +420,560 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>serial</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>UBNT20c040ff</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>edivaldosilva.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>UBNT20c04aa0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>faronildosilva</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>UBNT20c0a973</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>joellima1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>UBNT20c0b008</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ricardoangelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>UBNT29f0521f</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>antoniovieira</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>UBNT29f0650d</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>naircuerbas</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>UBNT29f084fb</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>maria_cabral.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UBNT29f5ffd3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>natielypeter</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>UBNT41309c70</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>josielnogueira</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>UBNT41317e94</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>dayane_martinhago.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>UBNT4131a180</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Juarez_francisco.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>UBNT4136c85c</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>jean_gomes.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UBNT4136dce4</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>emilly_andrade.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>UBNT4136dd4c</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>willianbrandao</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UBNT585a255c</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>transportadora_gs.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>UBNT585a260c</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>rafaeldasilva</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>UBNT585a26cc</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>alanramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UBNTb9062dc5</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>paulosh</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>UBNTb90637e3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>74:ac:b9:06:37:e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>UBNTb906c087</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>wandersonsporti-STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>UBNTb906c42a</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>casadacrianca</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>UBNTb906c4a8</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>jessicaberger1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>UBNTb906c551</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>inacio.silva_UNI</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UBNTb906cbf8</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>74:ac:b9:06:cb:f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>UBNTb906cbfc</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sandra_rodrigues.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>UBNTb906cbfd</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>allisonsilva</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>UBNTb906d8f3</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>escolapaulocherrer</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>UBNTb906ea4e</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>icaromoraes</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>UBNTb906ef74</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>valdeirmoura</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>UBNTb906f98f</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>daniela_santana.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>UBNTb906fb12</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>analesse</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>UBNTb9991b8c</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>LMC.10.NHDO.1527.DETRAN.810</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>UBNTb9991c06</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>henriquetravanci</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>UBNTb99927dc</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>aparecida_santos.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>UBNTe4e6639c</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>edsoncostancio</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>UBNTe4e6767a</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>rita_silva_UNI</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>UBNTe4e676e8</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>camilacongalves</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>UBNTf90b3a74</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>nboltda</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>UBNTf91a95c8</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>leandrorafasque1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>UBNTf91a9aa4</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>d0:21:f9:1a:9a:a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>UBNTf91ae1d8</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>paulodarocha</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>UBNTf91ae200</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>josemarques1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>UBNTf91ae450</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>marlucia_abelha.STM</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>UBNTf9a5a858</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>elisangeladasilva2</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>